<commit_message>
Finish groundwork and organize files
</commit_message>
<xml_diff>
--- a/data/ixis_assessment_table.xlsx
+++ b/data/ixis_assessment_table.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="month_device" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="month_diff" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="in_app" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -70,6 +71,27 @@
   </si>
   <si>
     <t xml:space="preserve">rd_atc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in_app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qpt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pct_sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pct_transactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pct_qty</t>
   </si>
 </sst>
 </file>
@@ -156,6 +178,28 @@
     <tableColumn id="12" name="rd_qty"/>
     <tableColumn id="13" name="d_atc"/>
     <tableColumn id="14" name="rd_atc"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:M72" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:M72"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="in_app"/>
+    <tableColumn id="2" name="dim_deviceCategory"/>
+    <tableColumn id="3" name="year"/>
+    <tableColumn id="4" name="month"/>
+    <tableColumn id="5" name="n"/>
+    <tableColumn id="6" name="sessions"/>
+    <tableColumn id="7" name="transactions"/>
+    <tableColumn id="8" name="qty"/>
+    <tableColumn id="9" name="tps"/>
+    <tableColumn id="10" name="qpt"/>
+    <tableColumn id="11" name="pct_sessions"/>
+    <tableColumn id="12" name="pct_transactions"/>
+    <tableColumn id="13" name="pct_qty"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1453,4 +1497,2973 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>193</v>
+      </c>
+      <c r="F2" t="n">
+        <v>335427</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10701</v>
+      </c>
+      <c r="H2" t="n">
+        <v>18547</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0319026196460035</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.73320250443884</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>217</v>
+      </c>
+      <c r="F3" t="n">
+        <v>392077</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12912</v>
+      </c>
+      <c r="H3" t="n">
+        <v>23316</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0329323066642522</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.80576208178439</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>192</v>
+      </c>
+      <c r="F4" t="n">
+        <v>272762</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8898</v>
+      </c>
+      <c r="H4" t="n">
+        <v>16507</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.03262184615159</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.85513598561474</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>204</v>
+      </c>
+      <c r="F5" t="n">
+        <v>302678</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9373</v>
+      </c>
+      <c r="H5" t="n">
+        <v>17675</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0309669021204052</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.8857356235997</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
+        <v>212</v>
+      </c>
+      <c r="F6" t="n">
+        <v>320717</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10350</v>
+      </c>
+      <c r="H6" t="n">
+        <v>18778</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0322714418007153</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.81429951690821</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="n">
+        <v>213</v>
+      </c>
+      <c r="F7" t="n">
+        <v>309717</v>
+      </c>
+      <c r="G7" t="n">
+        <v>11613</v>
+      </c>
+      <c r="H7" t="n">
+        <v>19947</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0374955201038367</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.71764401963317</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>209</v>
+      </c>
+      <c r="F8" t="n">
+        <v>393723</v>
+      </c>
+      <c r="G8" t="n">
+        <v>13793</v>
+      </c>
+      <c r="H8" t="n">
+        <v>25424</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0350322434808228</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.84325382440368</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>186</v>
+      </c>
+      <c r="F9" t="n">
+        <v>247625</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9699</v>
+      </c>
+      <c r="H9" t="n">
+        <v>18437</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0391680969207471</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.90091762037323</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>199</v>
+      </c>
+      <c r="F10" t="n">
+        <v>287828</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9679</v>
+      </c>
+      <c r="H10" t="n">
+        <v>17362</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0336277221118168</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.79378034920963</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>266</v>
+      </c>
+      <c r="F11" t="n">
+        <v>567506</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18868</v>
+      </c>
+      <c r="H11" t="n">
+        <v>34200</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0332472255799939</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.812592749629</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>277</v>
+      </c>
+      <c r="F12" t="n">
+        <v>526320</v>
+      </c>
+      <c r="G12" t="n">
+        <v>18176</v>
+      </c>
+      <c r="H12" t="n">
+        <v>33208</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0345341237270102</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.82702464788732</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>273</v>
+      </c>
+      <c r="F13" t="n">
+        <v>554929</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19370</v>
+      </c>
+      <c r="H13" t="n">
+        <v>35146</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0349053662720817</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.8144553433144</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D18" t="n">
+        <v>11</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J18" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>9</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D24" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7</v>
+      </c>
+      <c r="E25" t="n">
+        <v>209</v>
+      </c>
+      <c r="F25" t="n">
+        <v>251692</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2462</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4352</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.00978179679926259</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.7676685621446</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D26" t="n">
+        <v>8</v>
+      </c>
+      <c r="E26" t="n">
+        <v>207</v>
+      </c>
+      <c r="F26" t="n">
+        <v>252299</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3037</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5327</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0120373049437374</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.75403358577544</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" t="n">
+        <v>208</v>
+      </c>
+      <c r="F27" t="n">
+        <v>201203</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2284</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3926</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0113517194077623</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.71891418563923</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>197</v>
+      </c>
+      <c r="F28" t="n">
+        <v>211283</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2303</v>
+      </c>
+      <c r="H28" t="n">
+        <v>4269</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0109000724147234</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1.85366912722536</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D29" t="n">
+        <v>11</v>
+      </c>
+      <c r="E29" t="n">
+        <v>224</v>
+      </c>
+      <c r="F29" t="n">
+        <v>158167</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1877</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3191</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0118672036518364</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1.70005327650506</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D30" t="n">
+        <v>12</v>
+      </c>
+      <c r="E30" t="n">
+        <v>243</v>
+      </c>
+      <c r="F30" t="n">
+        <v>218756</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3075</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5554</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.0140567573003712</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.80617886178862</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>214</v>
+      </c>
+      <c r="F31" t="n">
+        <v>313673</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4259</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7098</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0135778342413915</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.66658840103311</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>193</v>
+      </c>
+      <c r="F32" t="n">
+        <v>167503</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1932</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3652</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.0115341217769234</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1.89026915113872</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>225</v>
+      </c>
+      <c r="F33" t="n">
+        <v>283268</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3528</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6280</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.0124546365985568</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1.78004535147392</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>286</v>
+      </c>
+      <c r="F34" t="n">
+        <v>384385</v>
+      </c>
+      <c r="G34" t="n">
+        <v>4110</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7456</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.0106924047504455</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1.81411192214112</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="b">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D35" t="n">
+        <v>5</v>
+      </c>
+      <c r="E35" t="n">
+        <v>281</v>
+      </c>
+      <c r="F35" t="n">
+        <v>373725</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5255</v>
+      </c>
+      <c r="H35" t="n">
+        <v>9518</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.0140611412134591</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1.81122740247383</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="b">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D36" t="n">
+        <v>6</v>
+      </c>
+      <c r="E36" t="n">
+        <v>303</v>
+      </c>
+      <c r="F36" t="n">
+        <v>479055</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7177</v>
+      </c>
+      <c r="H36" t="n">
+        <v>12645</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.0149815783156423</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1.76187822209837</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D37" t="n">
+        <v>7</v>
+      </c>
+      <c r="E37" t="n">
+        <v>20</v>
+      </c>
+      <c r="F37" t="n">
+        <v>22751</v>
+      </c>
+      <c r="G37" t="n">
+        <v>114</v>
+      </c>
+      <c r="H37" t="n">
+        <v>205</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.00501076875741726</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1.79824561403509</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D38" t="n">
+        <v>8</v>
+      </c>
+      <c r="E38" t="n">
+        <v>14</v>
+      </c>
+      <c r="F38" t="n">
+        <v>23257</v>
+      </c>
+      <c r="G38" t="n">
+        <v>128</v>
+      </c>
+      <c r="H38" t="n">
+        <v>245</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.00550371931031517</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1.9140625</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D39" t="n">
+        <v>9</v>
+      </c>
+      <c r="E39" t="n">
+        <v>14</v>
+      </c>
+      <c r="F39" t="n">
+        <v>19486</v>
+      </c>
+      <c r="G39" t="n">
+        <v>97</v>
+      </c>
+      <c r="H39" t="n">
+        <v>124</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.00497793287488453</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1.27835051546392</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D40" t="n">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>21</v>
+      </c>
+      <c r="F40" t="n">
+        <v>27566</v>
+      </c>
+      <c r="G40" t="n">
+        <v>115</v>
+      </c>
+      <c r="H40" t="n">
+        <v>177</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.0041718058477835</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1.53913043478261</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D41" t="n">
+        <v>11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>19</v>
+      </c>
+      <c r="F41" t="n">
+        <v>20661</v>
+      </c>
+      <c r="G41" t="n">
+        <v>117</v>
+      </c>
+      <c r="H41" t="n">
+        <v>216</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.00566284303760709</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1.84615384615385</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D42" t="n">
+        <v>12</v>
+      </c>
+      <c r="E42" t="n">
+        <v>14</v>
+      </c>
+      <c r="F42" t="n">
+        <v>15725</v>
+      </c>
+      <c r="G42" t="n">
+        <v>83</v>
+      </c>
+      <c r="H42" t="n">
+        <v>118</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.00527821939586645</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1.42168674698795</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>19</v>
+      </c>
+      <c r="F43" t="n">
+        <v>27995</v>
+      </c>
+      <c r="G43" t="n">
+        <v>101</v>
+      </c>
+      <c r="H43" t="n">
+        <v>159</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.00360778710484015</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1.57425742574257</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>20</v>
+      </c>
+      <c r="F44" t="n">
+        <v>27493</v>
+      </c>
+      <c r="G44" t="n">
+        <v>139</v>
+      </c>
+      <c r="H44" t="n">
+        <v>263</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.00505583239370021</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1.89208633093525</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" t="n">
+        <v>14</v>
+      </c>
+      <c r="F45" t="n">
+        <v>21564</v>
+      </c>
+      <c r="G45" t="n">
+        <v>116</v>
+      </c>
+      <c r="H45" t="n">
+        <v>175</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.00537933593025413</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1.50862068965517</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" t="n">
+        <v>23</v>
+      </c>
+      <c r="F46" t="n">
+        <v>45479</v>
+      </c>
+      <c r="G46" t="n">
+        <v>170</v>
+      </c>
+      <c r="H46" t="n">
+        <v>296</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.00373798896193848</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1.74117647058824</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D47" t="n">
+        <v>5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>23</v>
+      </c>
+      <c r="F47" t="n">
+        <v>36071</v>
+      </c>
+      <c r="G47" t="n">
+        <v>158</v>
+      </c>
+      <c r="H47" t="n">
+        <v>272</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.00438025006237698</v>
+      </c>
+      <c r="J47" t="n">
+        <v>1.72151898734177</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D48" t="n">
+        <v>6</v>
+      </c>
+      <c r="E48" t="n">
+        <v>22</v>
+      </c>
+      <c r="F48" t="n">
+        <v>47426</v>
+      </c>
+      <c r="G48" t="n">
+        <v>235</v>
+      </c>
+      <c r="H48" t="n">
+        <v>372</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.00495508792645384</v>
+      </c>
+      <c r="J48" t="n">
+        <v>1.58297872340426</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="b">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D49" t="n">
+        <v>7</v>
+      </c>
+      <c r="E49" t="n">
+        <v>140</v>
+      </c>
+      <c r="F49" t="n">
+        <v>145335</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4778</v>
+      </c>
+      <c r="H49" t="n">
+        <v>8544</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.0328757697732824</v>
+      </c>
+      <c r="J49" t="n">
+        <v>1.78819589786522</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D50" t="n">
+        <v>8</v>
+      </c>
+      <c r="E50" t="n">
+        <v>138</v>
+      </c>
+      <c r="F50" t="n">
+        <v>140049</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3124</v>
+      </c>
+      <c r="H50" t="n">
+        <v>5623</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.0223064784468293</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1.79993597951344</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D51" t="n">
+        <v>9</v>
+      </c>
+      <c r="E51" t="n">
+        <v>133</v>
+      </c>
+      <c r="F51" t="n">
+        <v>159163</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4281</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7740</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.0268969546942443</v>
+      </c>
+      <c r="J51" t="n">
+        <v>1.80798878766643</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="b">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D52" t="n">
+        <v>10</v>
+      </c>
+      <c r="E52" t="n">
+        <v>148</v>
+      </c>
+      <c r="F52" t="n">
+        <v>94205</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2398</v>
+      </c>
+      <c r="H52" t="n">
+        <v>4367</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.0254551244626081</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1.82110091743119</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D53" t="n">
+        <v>11</v>
+      </c>
+      <c r="E53" t="n">
+        <v>126</v>
+      </c>
+      <c r="F53" t="n">
+        <v>121642</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3064</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5794</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.0251886683875635</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1.89099216710183</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="b">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D54" t="n">
+        <v>12</v>
+      </c>
+      <c r="E54" t="n">
+        <v>142</v>
+      </c>
+      <c r="F54" t="n">
+        <v>233341</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5045</v>
+      </c>
+      <c r="H54" t="n">
+        <v>8935</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.0216207181764028</v>
+      </c>
+      <c r="J54" t="n">
+        <v>1.77106045589693</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="b">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>151</v>
+      </c>
+      <c r="F55" t="n">
+        <v>151553</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3315</v>
+      </c>
+      <c r="H55" t="n">
+        <v>5984</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.0218735359907095</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1.80512820512821</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="n">
+        <v>125</v>
+      </c>
+      <c r="F56" t="n">
+        <v>99970</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2345</v>
+      </c>
+      <c r="H56" t="n">
+        <v>4583</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.0234570371111333</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1.9543710021322</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" t="n">
+        <v>143</v>
+      </c>
+      <c r="F57" t="n">
+        <v>182258</v>
+      </c>
+      <c r="G57" t="n">
+        <v>4360</v>
+      </c>
+      <c r="H57" t="n">
+        <v>8094</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.0239221323618168</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1.85642201834862</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="b">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D58" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" t="n">
+        <v>186</v>
+      </c>
+      <c r="F58" t="n">
+        <v>272961</v>
+      </c>
+      <c r="G58" t="n">
+        <v>6964</v>
+      </c>
+      <c r="H58" t="n">
+        <v>12546</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.0255128021951854</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1.80155083285468</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="b">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D59" t="n">
+        <v>5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>195</v>
+      </c>
+      <c r="F59" t="n">
+        <v>206169</v>
+      </c>
+      <c r="G59" t="n">
+        <v>4616</v>
+      </c>
+      <c r="H59" t="n">
+        <v>8292</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.0223893989882087</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1.79636048526863</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="b">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D60" t="n">
+        <v>6</v>
+      </c>
+      <c r="E60" t="n">
+        <v>200</v>
+      </c>
+      <c r="F60" t="n">
+        <v>287376</v>
+      </c>
+      <c r="G60" t="n">
+        <v>7588</v>
+      </c>
+      <c r="H60" t="n">
+        <v>13400</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.0264044318245087</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1.76594623089088</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="b">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D61" t="n">
+        <v>7</v>
+      </c>
+      <c r="E61" t="n">
+        <v>17</v>
+      </c>
+      <c r="F61" t="n">
+        <v>13382</v>
+      </c>
+      <c r="G61" t="n">
+        <v>106</v>
+      </c>
+      <c r="H61" t="n">
+        <v>156</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.00792108802869526</v>
+      </c>
+      <c r="J61" t="n">
+        <v>1.47169811320755</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D62" t="n">
+        <v>8</v>
+      </c>
+      <c r="E62" t="n">
+        <v>19</v>
+      </c>
+      <c r="F62" t="n">
+        <v>14809</v>
+      </c>
+      <c r="G62" t="n">
+        <v>78</v>
+      </c>
+      <c r="H62" t="n">
+        <v>137</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.00526706732392464</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1.75641025641026</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="b">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D63" t="n">
+        <v>9</v>
+      </c>
+      <c r="E63" t="n">
+        <v>13</v>
+      </c>
+      <c r="F63" t="n">
+        <v>10030</v>
+      </c>
+      <c r="G63" t="n">
+        <v>98</v>
+      </c>
+      <c r="H63" t="n">
+        <v>129</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.00977068793619143</v>
+      </c>
+      <c r="J63" t="n">
+        <v>1.31632653061224</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="b">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D64" t="n">
+        <v>10</v>
+      </c>
+      <c r="E64" t="n">
+        <v>18</v>
+      </c>
+      <c r="F64" t="n">
+        <v>12903</v>
+      </c>
+      <c r="G64" t="n">
+        <v>86</v>
+      </c>
+      <c r="H64" t="n">
+        <v>138</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.00666511663954119</v>
+      </c>
+      <c r="J64" t="n">
+        <v>1.6046511627907</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="b">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D65" t="n">
+        <v>11</v>
+      </c>
+      <c r="E65" t="n">
+        <v>18</v>
+      </c>
+      <c r="F65" t="n">
+        <v>16593</v>
+      </c>
+      <c r="G65" t="n">
+        <v>119</v>
+      </c>
+      <c r="H65" t="n">
+        <v>153</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.00717169890917857</v>
+      </c>
+      <c r="J65" t="n">
+        <v>1.28571428571429</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D66" t="n">
+        <v>12</v>
+      </c>
+      <c r="E66" t="n">
+        <v>15</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12094</v>
+      </c>
+      <c r="G66" t="n">
+        <v>113</v>
+      </c>
+      <c r="H66" t="n">
+        <v>198</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.00934347610385315</v>
+      </c>
+      <c r="J66" t="n">
+        <v>1.75221238938053</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="b">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>19</v>
+      </c>
+      <c r="F67" t="n">
+        <v>13048</v>
+      </c>
+      <c r="G67" t="n">
+        <v>92</v>
+      </c>
+      <c r="H67" t="n">
+        <v>181</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.00705088902513795</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1.96739130434783</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="b">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E68" t="n">
+        <v>15</v>
+      </c>
+      <c r="F68" t="n">
+        <v>7629</v>
+      </c>
+      <c r="G68" t="n">
+        <v>51</v>
+      </c>
+      <c r="H68" t="n">
+        <v>113</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.00668501769563508</v>
+      </c>
+      <c r="J68" t="n">
+        <v>2.2156862745098</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="b">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3</v>
+      </c>
+      <c r="E69" t="n">
+        <v>20</v>
+      </c>
+      <c r="F69" t="n">
+        <v>13893</v>
+      </c>
+      <c r="G69" t="n">
+        <v>121</v>
+      </c>
+      <c r="H69" t="n">
+        <v>171</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.00870942201108472</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1.41322314049587</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="b">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D70" t="n">
+        <v>4</v>
+      </c>
+      <c r="E70" t="n">
+        <v>26</v>
+      </c>
+      <c r="F70" t="n">
+        <v>26278</v>
+      </c>
+      <c r="G70" t="n">
+        <v>257</v>
+      </c>
+      <c r="H70" t="n">
+        <v>448</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.00978004414338991</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1.7431906614786</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D71" t="n">
+        <v>5</v>
+      </c>
+      <c r="E71" t="n">
+        <v>19</v>
+      </c>
+      <c r="F71" t="n">
+        <v>22344</v>
+      </c>
+      <c r="G71" t="n">
+        <v>184</v>
+      </c>
+      <c r="H71" t="n">
+        <v>339</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.00823487289652703</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1.84239130434783</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="b">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D72" t="n">
+        <v>6</v>
+      </c>
+      <c r="E72" t="n">
+        <v>23</v>
+      </c>
+      <c r="F72" t="n">
+        <v>20037</v>
+      </c>
+      <c r="G72" t="n">
+        <v>168</v>
+      </c>
+      <c r="H72" t="n">
+        <v>328</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.00838448869591256</v>
+      </c>
+      <c r="J72" t="n">
+        <v>1.95238095238095</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update code commenting, clean up a little
</commit_message>
<xml_diff>
--- a/data/ixis_assessment_table.xlsx
+++ b/data/ixis_assessment_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -49,6 +49,12 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">d_ecr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd_ecr</t>
+  </si>
+  <si>
     <t xml:space="preserve">d_sessions</t>
   </si>
   <si>
@@ -77,21 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qpt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pct_sessions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pct_transactions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pct_qty</t>
   </si>
 </sst>
 </file>
@@ -161,32 +152,35 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N3"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:Q3"/>
+  <tableColumns count="17">
     <tableColumn id="1" name="date"/>
     <tableColumn id="2" name="year"/>
     <tableColumn id="3" name="month"/>
-    <tableColumn id="4" name="sessions"/>
-    <tableColumn id="5" name="d_sessions"/>
-    <tableColumn id="6" name="rd_sessions"/>
-    <tableColumn id="7" name="transactions"/>
-    <tableColumn id="8" name="d_transactions"/>
-    <tableColumn id="9" name="rd_transactions"/>
-    <tableColumn id="10" name="qty"/>
-    <tableColumn id="11" name="d_qty"/>
-    <tableColumn id="12" name="rd_qty"/>
-    <tableColumn id="13" name="d_atc"/>
-    <tableColumn id="14" name="rd_atc"/>
+    <tableColumn id="4" name="ecr"/>
+    <tableColumn id="5" name="d_ecr"/>
+    <tableColumn id="6" name="rd_ecr"/>
+    <tableColumn id="7" name="sessions"/>
+    <tableColumn id="8" name="d_sessions"/>
+    <tableColumn id="9" name="rd_sessions"/>
+    <tableColumn id="10" name="transactions"/>
+    <tableColumn id="11" name="d_transactions"/>
+    <tableColumn id="12" name="rd_transactions"/>
+    <tableColumn id="13" name="qty"/>
+    <tableColumn id="14" name="d_qty"/>
+    <tableColumn id="15" name="rd_qty"/>
+    <tableColumn id="16" name="d_atc"/>
+    <tableColumn id="17" name="rd_atc"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:M72" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:M72"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I72" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I72"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="in_app"/>
     <tableColumn id="2" name="dim_deviceCategory"/>
     <tableColumn id="3" name="year"/>
@@ -195,11 +189,7 @@
     <tableColumn id="6" name="sessions"/>
     <tableColumn id="7" name="transactions"/>
     <tableColumn id="8" name="qty"/>
-    <tableColumn id="9" name="tps"/>
-    <tableColumn id="10" name="qpt"/>
-    <tableColumn id="11" name="pct_sessions"/>
-    <tableColumn id="12" name="pct_transactions"/>
-    <tableColumn id="13" name="pct_qty"/>
+    <tableColumn id="9" name="ecr"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -1378,7 +1368,7 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
         <v>13</v>
@@ -1387,7 +1377,7 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
@@ -1396,10 +1386,19 @@
         <v>16</v>
       </c>
       <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1413,36 +1412,45 @@
         <v>5</v>
       </c>
       <c r="D2" t="n">
+        <v>0.113712923834892</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.0079309447036911</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.0651980638150746</v>
+      </c>
+      <c r="G2" t="n">
         <v>1164639</v>
       </c>
-      <c r="E2" t="n">
+      <c r="H2" t="n">
         <v>-131974</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>-0.101783647086679</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>28389</v>
       </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
         <v>-1980</v>
       </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>-0.0651980638150746</v>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>51629</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>-3317</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
         <v>-0.0603683616641794</v>
       </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
         <v>-47122</v>
       </c>
-      <c r="N2" t="n">
+      <c r="Q2" t="n">
         <v>-0.256317925174878</v>
       </c>
     </row>
@@ -1457,36 +1465,45 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
+        <v>0.138342913220244</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0246299893853518</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.216597978090105</v>
+      </c>
+      <c r="G3" t="n">
         <v>1388834</v>
       </c>
-      <c r="E3" t="n">
+      <c r="H3" t="n">
         <v>224195</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>0.192501710830566</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>34538</v>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>6149</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.216597978090105</v>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>61891</v>
       </c>
-      <c r="K3" t="n">
+      <c r="N3" t="n">
         <v>10262</v>
       </c>
-      <c r="L3" t="n">
+      <c r="O3" t="n">
         <v>0.198764260396289</v>
       </c>
-      <c r="M3" t="n">
+      <c r="P3" t="n">
         <v>-28750</v>
       </c>
-      <c r="N3" t="n">
+      <c r="Q3" t="n">
         <v>-0.210283791691047</v>
       </c>
     </row>
@@ -1509,7 +1526,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1521,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1533,19 +1550,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -1576,18 +1581,6 @@
       <c r="I2" t="n">
         <v>0.0319026196460035</v>
       </c>
-      <c r="J2" t="n">
-        <v>1.73320250443884</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="b">
@@ -1617,18 +1610,6 @@
       <c r="I3" t="n">
         <v>0.0329323066642522</v>
       </c>
-      <c r="J3" t="n">
-        <v>1.80576208178439</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="b">
@@ -1658,18 +1639,6 @@
       <c r="I4" t="n">
         <v>0.03262184615159</v>
       </c>
-      <c r="J4" t="n">
-        <v>1.85513598561474</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="b">
@@ -1699,18 +1668,6 @@
       <c r="I5" t="n">
         <v>0.0309669021204052</v>
       </c>
-      <c r="J5" t="n">
-        <v>1.8857356235997</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="b">
@@ -1740,18 +1697,6 @@
       <c r="I6" t="n">
         <v>0.0322714418007153</v>
       </c>
-      <c r="J6" t="n">
-        <v>1.81429951690821</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -1781,18 +1726,6 @@
       <c r="I7" t="n">
         <v>0.0374955201038367</v>
       </c>
-      <c r="J7" t="n">
-        <v>1.71764401963317</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="b">
@@ -1822,18 +1755,6 @@
       <c r="I8" t="n">
         <v>0.0350322434808228</v>
       </c>
-      <c r="J8" t="n">
-        <v>1.84325382440368</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="b">
@@ -1863,18 +1784,6 @@
       <c r="I9" t="n">
         <v>0.0391680969207471</v>
       </c>
-      <c r="J9" t="n">
-        <v>1.90091762037323</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="b">
@@ -1904,18 +1813,6 @@
       <c r="I10" t="n">
         <v>0.0336277221118168</v>
       </c>
-      <c r="J10" t="n">
-        <v>1.79378034920963</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -1945,18 +1842,6 @@
       <c r="I11" t="n">
         <v>0.0332472255799939</v>
       </c>
-      <c r="J11" t="n">
-        <v>1.812592749629</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.12</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -1986,18 +1871,6 @@
       <c r="I12" t="n">
         <v>0.0345341237270102</v>
       </c>
-      <c r="J12" t="n">
-        <v>1.82702464788732</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.12</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="b">
@@ -2027,18 +1900,6 @@
       <c r="I13" t="n">
         <v>0.0349053662720817</v>
       </c>
-      <c r="J13" t="n">
-        <v>1.8144553433144</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.13</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="b">
@@ -2068,18 +1929,6 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -2109,18 +1958,6 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="b">
@@ -2150,18 +1987,6 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="J16" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="b">
@@ -2191,18 +2016,6 @@
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="b">
@@ -2232,18 +2045,6 @@
       <c r="I18" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="J18" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -2273,18 +2074,6 @@
       <c r="I19" t="n">
         <v>0</v>
       </c>
-      <c r="J19" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="b">
@@ -2314,18 +2103,6 @@
       <c r="I20" t="n">
         <v>0</v>
       </c>
-      <c r="J20" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="b">
@@ -2355,18 +2132,6 @@
       <c r="I21" t="n">
         <v>0</v>
       </c>
-      <c r="J21" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="b">
@@ -2396,18 +2161,6 @@
       <c r="I22" t="n">
         <v>0</v>
       </c>
-      <c r="J22" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="b">
@@ -2437,18 +2190,6 @@
       <c r="I23" t="n">
         <v>0</v>
       </c>
-      <c r="J23" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="b">
@@ -2478,18 +2219,6 @@
       <c r="I24" t="n">
         <v>0</v>
       </c>
-      <c r="J24" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="b">
@@ -2519,18 +2248,6 @@
       <c r="I25" t="n">
         <v>0.00978179679926259</v>
       </c>
-      <c r="J25" t="n">
-        <v>1.7676685621446</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="b">
@@ -2560,18 +2277,6 @@
       <c r="I26" t="n">
         <v>0.0120373049437374</v>
       </c>
-      <c r="J26" t="n">
-        <v>1.75403358577544</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="b">
@@ -2601,18 +2306,6 @@
       <c r="I27" t="n">
         <v>0.0113517194077623</v>
       </c>
-      <c r="J27" t="n">
-        <v>1.71891418563923</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="b">
@@ -2642,18 +2335,6 @@
       <c r="I28" t="n">
         <v>0.0109000724147234</v>
       </c>
-      <c r="J28" t="n">
-        <v>1.85366912722536</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="b">
@@ -2683,18 +2364,6 @@
       <c r="I29" t="n">
         <v>0.0118672036518364</v>
       </c>
-      <c r="J29" t="n">
-        <v>1.70005327650506</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0.04</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="b">
@@ -2724,18 +2393,6 @@
       <c r="I30" t="n">
         <v>0.0140567573003712</v>
       </c>
-      <c r="J30" t="n">
-        <v>1.80617886178862</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0.07</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="b">
@@ -2765,18 +2422,6 @@
       <c r="I31" t="n">
         <v>0.0135778342413915</v>
       </c>
-      <c r="J31" t="n">
-        <v>1.66658840103311</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="b">
@@ -2806,18 +2451,6 @@
       <c r="I32" t="n">
         <v>0.0115341217769234</v>
       </c>
-      <c r="J32" t="n">
-        <v>1.89026915113872</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="b">
@@ -2847,18 +2480,6 @@
       <c r="I33" t="n">
         <v>0.0124546365985568</v>
       </c>
-      <c r="J33" t="n">
-        <v>1.78004535147392</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="b">
@@ -2888,18 +2509,6 @@
       <c r="I34" t="n">
         <v>0.0106924047504455</v>
       </c>
-      <c r="J34" t="n">
-        <v>1.81411192214112</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="b">
@@ -2929,18 +2538,6 @@
       <c r="I35" t="n">
         <v>0.0140611412134591</v>
       </c>
-      <c r="J35" t="n">
-        <v>1.81122740247383</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.13</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="b">
@@ -2970,18 +2567,6 @@
       <c r="I36" t="n">
         <v>0.0149815783156423</v>
       </c>
-      <c r="J36" t="n">
-        <v>1.76187822209837</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0.17</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="b">
@@ -3011,18 +2596,6 @@
       <c r="I37" t="n">
         <v>0.00501076875741726</v>
       </c>
-      <c r="J37" t="n">
-        <v>1.79824561403509</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="b">
@@ -3052,18 +2625,6 @@
       <c r="I38" t="n">
         <v>0.00550371931031517</v>
       </c>
-      <c r="J38" t="n">
-        <v>1.9140625</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="b">
@@ -3093,18 +2654,6 @@
       <c r="I39" t="n">
         <v>0.00497793287488453</v>
       </c>
-      <c r="J39" t="n">
-        <v>1.27835051546392</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="b">
@@ -3134,18 +2683,6 @@
       <c r="I40" t="n">
         <v>0.0041718058477835</v>
       </c>
-      <c r="J40" t="n">
-        <v>1.53913043478261</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="b">
@@ -3175,18 +2712,6 @@
       <c r="I41" t="n">
         <v>0.00566284303760709</v>
       </c>
-      <c r="J41" t="n">
-        <v>1.84615384615385</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="b">
@@ -3216,18 +2741,6 @@
       <c r="I42" t="n">
         <v>0.00527821939586645</v>
       </c>
-      <c r="J42" t="n">
-        <v>1.42168674698795</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="b">
@@ -3257,18 +2770,6 @@
       <c r="I43" t="n">
         <v>0.00360778710484015</v>
       </c>
-      <c r="J43" t="n">
-        <v>1.57425742574257</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="b">
@@ -3298,18 +2799,6 @@
       <c r="I44" t="n">
         <v>0.00505583239370021</v>
       </c>
-      <c r="J44" t="n">
-        <v>1.89208633093525</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="b">
@@ -3339,18 +2828,6 @@
       <c r="I45" t="n">
         <v>0.00537933593025413</v>
       </c>
-      <c r="J45" t="n">
-        <v>1.50862068965517</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="b">
@@ -3380,18 +2857,6 @@
       <c r="I46" t="n">
         <v>0.00373798896193848</v>
       </c>
-      <c r="J46" t="n">
-        <v>1.74117647058824</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="b">
@@ -3421,18 +2886,6 @@
       <c r="I47" t="n">
         <v>0.00438025006237698</v>
       </c>
-      <c r="J47" t="n">
-        <v>1.72151898734177</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="b">
@@ -3462,18 +2915,6 @@
       <c r="I48" t="n">
         <v>0.00495508792645384</v>
       </c>
-      <c r="J48" t="n">
-        <v>1.58297872340426</v>
-      </c>
-      <c r="K48" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M48" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="b">
@@ -3503,18 +2944,6 @@
       <c r="I49" t="n">
         <v>0.0328757697732824</v>
       </c>
-      <c r="J49" t="n">
-        <v>1.78819589786522</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M49" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="b">
@@ -3544,18 +2973,6 @@
       <c r="I50" t="n">
         <v>0.0223064784468293</v>
       </c>
-      <c r="J50" t="n">
-        <v>1.79993597951344</v>
-      </c>
-      <c r="K50" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="b">
@@ -3585,18 +3002,6 @@
       <c r="I51" t="n">
         <v>0.0268969546942443</v>
       </c>
-      <c r="J51" t="n">
-        <v>1.80798878766643</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="M51" t="n">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="b">
@@ -3626,18 +3031,6 @@
       <c r="I52" t="n">
         <v>0.0254551244626081</v>
       </c>
-      <c r="J52" t="n">
-        <v>1.82110091743119</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="M52" t="n">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="b">
@@ -3667,18 +3060,6 @@
       <c r="I53" t="n">
         <v>0.0251886683875635</v>
       </c>
-      <c r="J53" t="n">
-        <v>1.89099216710183</v>
-      </c>
-      <c r="K53" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="L53" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M53" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="b">
@@ -3708,18 +3089,6 @@
       <c r="I54" t="n">
         <v>0.0216207181764028</v>
       </c>
-      <c r="J54" t="n">
-        <v>1.77106045589693</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="b">
@@ -3749,18 +3118,6 @@
       <c r="I55" t="n">
         <v>0.0218735359907095</v>
       </c>
-      <c r="J55" t="n">
-        <v>1.80512820512821</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0.06</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="b">
@@ -3790,18 +3147,6 @@
       <c r="I56" t="n">
         <v>0.0234570371111333</v>
       </c>
-      <c r="J56" t="n">
-        <v>1.9543710021322</v>
-      </c>
-      <c r="K56" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="b">
@@ -3831,18 +3176,6 @@
       <c r="I57" t="n">
         <v>0.0239221323618168</v>
       </c>
-      <c r="J57" t="n">
-        <v>1.85642201834862</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="M57" t="n">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="b">
@@ -3872,18 +3205,6 @@
       <c r="I58" t="n">
         <v>0.0255128021951854</v>
       </c>
-      <c r="J58" t="n">
-        <v>1.80155083285468</v>
-      </c>
-      <c r="K58" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="L58" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0.13</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="b">
@@ -3913,18 +3234,6 @@
       <c r="I59" t="n">
         <v>0.0223893989882087</v>
       </c>
-      <c r="J59" t="n">
-        <v>1.79636048526863</v>
-      </c>
-      <c r="K59" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="L59" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M59" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="b">
@@ -3954,18 +3263,6 @@
       <c r="I60" t="n">
         <v>0.0264044318245087</v>
       </c>
-      <c r="J60" t="n">
-        <v>1.76594623089088</v>
-      </c>
-      <c r="K60" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="L60" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="M60" t="n">
-        <v>0.14</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="b">
@@ -3995,18 +3292,6 @@
       <c r="I61" t="n">
         <v>0.00792108802869526</v>
       </c>
-      <c r="J61" t="n">
-        <v>1.47169811320755</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="b">
@@ -4036,18 +3321,6 @@
       <c r="I62" t="n">
         <v>0.00526706732392464</v>
       </c>
-      <c r="J62" t="n">
-        <v>1.75641025641026</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="b">
@@ -4077,18 +3350,6 @@
       <c r="I63" t="n">
         <v>0.00977068793619143</v>
       </c>
-      <c r="J63" t="n">
-        <v>1.31632653061224</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0</v>
-      </c>
-      <c r="L63" t="n">
-        <v>0</v>
-      </c>
-      <c r="M63" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="b">
@@ -4118,18 +3379,6 @@
       <c r="I64" t="n">
         <v>0.00666511663954119</v>
       </c>
-      <c r="J64" t="n">
-        <v>1.6046511627907</v>
-      </c>
-      <c r="K64" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="b">
@@ -4159,18 +3408,6 @@
       <c r="I65" t="n">
         <v>0.00717169890917857</v>
       </c>
-      <c r="J65" t="n">
-        <v>1.28571428571429</v>
-      </c>
-      <c r="K65" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0</v>
-      </c>
-      <c r="M65" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="b">
@@ -4200,18 +3437,6 @@
       <c r="I66" t="n">
         <v>0.00934347610385315</v>
       </c>
-      <c r="J66" t="n">
-        <v>1.75221238938053</v>
-      </c>
-      <c r="K66" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="b">
@@ -4241,18 +3466,6 @@
       <c r="I67" t="n">
         <v>0.00705088902513795</v>
       </c>
-      <c r="J67" t="n">
-        <v>1.96739130434783</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="b">
@@ -4282,18 +3495,6 @@
       <c r="I68" t="n">
         <v>0.00668501769563508</v>
       </c>
-      <c r="J68" t="n">
-        <v>2.2156862745098</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="b">
@@ -4323,18 +3524,6 @@
       <c r="I69" t="n">
         <v>0.00870942201108472</v>
       </c>
-      <c r="J69" t="n">
-        <v>1.41322314049587</v>
-      </c>
-      <c r="K69" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L69" t="n">
-        <v>0</v>
-      </c>
-      <c r="M69" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="b">
@@ -4364,18 +3553,6 @@
       <c r="I70" t="n">
         <v>0.00978004414338991</v>
       </c>
-      <c r="J70" t="n">
-        <v>1.7431906614786</v>
-      </c>
-      <c r="K70" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L70" t="n">
-        <v>0</v>
-      </c>
-      <c r="M70" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="b">
@@ -4405,18 +3582,6 @@
       <c r="I71" t="n">
         <v>0.00823487289652703</v>
       </c>
-      <c r="J71" t="n">
-        <v>1.84239130434783</v>
-      </c>
-      <c r="K71" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L71" t="n">
-        <v>0</v>
-      </c>
-      <c r="M71" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="b">
@@ -4445,18 +3610,6 @@
       </c>
       <c r="I72" t="n">
         <v>0.00838448869591256</v>
-      </c>
-      <c r="J72" t="n">
-        <v>1.95238095238095</v>
-      </c>
-      <c r="K72" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L72" t="n">
-        <v>0</v>
-      </c>
-      <c r="M72" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>